<commit_message>
speriamo, vedo se modifiche funzionano, ho aggiunto sottosezioni
</commit_message>
<xml_diff>
--- a/output/blocchi_multi_foglio.xlsx
+++ b/output/blocchi_multi_foglio.xlsx
@@ -1425,12 +1425,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>542609</t>
+          <t>537153</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>V.le delle Americhe  48122 Ravenna ( RA )</t>
+          <t>Via delle Americhe  48122 Ravenna ( RA )</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1460,12 +1460,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>537153</t>
+          <t>542609</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Via delle Americhe  48122 Ravenna ( RA )</t>
+          <t>V.le delle Americhe  48122 Ravenna ( RA )</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">

</xml_diff>